<commit_message>
Apply everything to Amy's cases
Checked through and fixed lots of little bugs in adapting code
</commit_message>
<xml_diff>
--- a/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
+++ b/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="1340" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="41">
   <si>
     <t>Whale ID</t>
   </si>
@@ -111,9 +111,6 @@
     <t>J092609-1</t>
   </si>
   <si>
-    <t>Gear length info from PCCS Page</t>
-  </si>
-  <si>
     <t>Auxiliary wetted area (m^3)</t>
   </si>
   <si>
@@ -127,6 +124,24 @@
   </si>
   <si>
     <t>Lobster trap CD = 2, buoy = 0.6, so said 1.8 (estimated weighted average)</t>
+  </si>
+  <si>
+    <t>Whale Age</t>
+  </si>
+  <si>
+    <t>20+</t>
+  </si>
+  <si>
+    <t>17+</t>
+  </si>
+  <si>
+    <t>Gear length info from PCCS Page; Lobster trap</t>
+  </si>
+  <si>
+    <t>pApt</t>
+  </si>
+  <si>
+    <t>Y</t>
   </si>
 </sst>
 </file>
@@ -184,8 +199,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -207,7 +234,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="27">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -215,6 +242,12 @@
     <cellStyle name="Followed Hyperlink" xfId="10" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="12" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="14" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="16" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="18" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="20" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="22" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="24" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="26" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -222,6 +255,12 @@
     <cellStyle name="Hyperlink" xfId="9" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="11" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="13" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="15" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="17" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="19" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="21" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="23" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="25" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -551,15 +590,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:I16"/>
+  <dimension ref="A1:K16"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L17" sqref="L17"/>
+      <selection activeCell="K15" sqref="K15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:11">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -573,22 +612,28 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H1" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="2" spans="1:9">
+      <c r="J1" t="s">
+        <v>35</v>
+      </c>
+      <c r="K1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11">
       <c r="A2">
         <v>1238</v>
       </c>
@@ -608,10 +653,16 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9">
+        <v>31</v>
+      </c>
+      <c r="J2" t="s">
+        <v>36</v>
+      </c>
+      <c r="K2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11">
       <c r="A3">
         <v>1427</v>
       </c>
@@ -636,8 +687,14 @@
       <c r="H3">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="4" spans="1:9">
+      <c r="J3">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11">
       <c r="A4">
         <v>1971</v>
       </c>
@@ -662,8 +719,14 @@
       <c r="H4">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="5" spans="1:9">
+      <c r="J4">
+        <v>8</v>
+      </c>
+      <c r="K4" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11">
       <c r="A5">
         <v>2027</v>
       </c>
@@ -686,10 +749,16 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9">
+        <v>31</v>
+      </c>
+      <c r="J5">
+        <v>7</v>
+      </c>
+      <c r="K5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11">
       <c r="A6">
         <v>2151</v>
       </c>
@@ -709,10 +778,16 @@
         <v>0</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" s="1" customFormat="1">
+        <v>31</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" s="1" customFormat="1">
       <c r="A7" s="1">
         <v>2223</v>
       </c>
@@ -735,10 +810,16 @@
         <v>0</v>
       </c>
       <c r="H7" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" s="1" customFormat="1">
+        <v>31</v>
+      </c>
+      <c r="J7" s="1">
+        <v>8</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" s="1" customFormat="1">
       <c r="A8" s="1">
         <v>2427</v>
       </c>
@@ -763,8 +844,14 @@
       <c r="H8" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="9" spans="1:9" s="1" customFormat="1">
+      <c r="J8" s="1">
+        <v>7</v>
+      </c>
+      <c r="K8" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" s="1" customFormat="1">
       <c r="A9" s="1">
         <v>2470</v>
       </c>
@@ -784,13 +871,19 @@
         <v>0</v>
       </c>
       <c r="H9" s="1" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I9" s="1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="10" spans="1:9" s="1" customFormat="1">
+      <c r="J9" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="K9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" s="1" customFormat="1">
       <c r="A10" s="1">
         <v>2753</v>
       </c>
@@ -815,8 +908,14 @@
       <c r="H10" s="1">
         <v>0.5</v>
       </c>
-    </row>
-    <row r="11" spans="1:9" s="1" customFormat="1">
+      <c r="J10" s="1">
+        <v>2</v>
+      </c>
+      <c r="K10" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" s="1" customFormat="1">
       <c r="A11" s="1">
         <v>3120</v>
       </c>
@@ -841,8 +940,14 @@
       <c r="H11" s="1">
         <v>0.6</v>
       </c>
-    </row>
-    <row r="12" spans="1:9" s="1" customFormat="1">
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" s="1" customFormat="1">
       <c r="A12" s="1">
         <v>3392</v>
       </c>
@@ -868,10 +973,16 @@
         <v>1.8</v>
       </c>
       <c r="I12" s="1" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" s="1" customFormat="1">
+        <v>34</v>
+      </c>
+      <c r="J12" s="1">
+        <v>1</v>
+      </c>
+      <c r="K12" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" s="1" customFormat="1">
       <c r="A13" s="1">
         <v>3420</v>
       </c>
@@ -894,10 +1005,16 @@
         <v>0</v>
       </c>
       <c r="H13" s="1" t="s">
-        <v>32</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" s="2" customFormat="1">
+        <v>31</v>
+      </c>
+      <c r="J13" s="1">
+        <v>5</v>
+      </c>
+      <c r="K13" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" s="2" customFormat="1">
       <c r="A14" s="2">
         <v>3821</v>
       </c>
@@ -923,17 +1040,23 @@
         <v>2</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9">
+        <v>38</v>
+      </c>
+      <c r="J14" s="2">
+        <v>1</v>
+      </c>
+      <c r="K14" s="2" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11">
       <c r="A15" s="3"/>
       <c r="D15" s="3"/>
       <c r="F15" s="3"/>
       <c r="G15" s="3"/>
       <c r="H15" s="3"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:11">
       <c r="D16" s="3"/>
       <c r="F16" s="3"/>
       <c r="G16" s="3"/>

</xml_diff>

<commit_message>
Only 11 cases from ARK
</commit_message>
<xml_diff>
--- a/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
+++ b/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25600" windowHeight="14880" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$V$14</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
   </definedNames>
   <calcPr calcId="140000" concurrentCalc="0"/>
   <extLst>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="87" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
   <si>
     <t>Whale ID</t>
   </si>
@@ -66,12 +66,6 @@
     <t>J111694</t>
   </si>
   <si>
-    <t>E24-00</t>
-  </si>
-  <si>
-    <t>J081800</t>
-  </si>
-  <si>
     <t>E09-01</t>
   </si>
   <si>
@@ -102,12 +96,6 @@
     <t>J070903</t>
   </si>
   <si>
-    <t>E02-09</t>
-  </si>
-  <si>
-    <t>J013109</t>
-  </si>
-  <si>
     <t>E25-09</t>
   </si>
   <si>
@@ -130,12 +118,6 @@
   </si>
   <si>
     <t>Whale Age</t>
-  </si>
-  <si>
-    <t>20+</t>
-  </si>
-  <si>
-    <t>17+</t>
   </si>
   <si>
     <t>Gear length info from PCCS Page; Lobster trap</t>
@@ -265,8 +247,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="33">
+  <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -311,7 +309,7 @@
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="33">
+  <cellStyles count="49">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -328,6 +326,14 @@
     <cellStyle name="Followed Hyperlink" xfId="28" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="30" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="32" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="34" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="36" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="38" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="40" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="42" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -344,6 +350,14 @@
     <cellStyle name="Hyperlink" xfId="27" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="29" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="31" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="33" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="35" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="37" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="39" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="41" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -673,10 +687,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z16"/>
+  <dimension ref="A1:Z14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="J1" workbookViewId="0">
-      <selection activeCell="X18" sqref="X18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J9" sqref="J9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -695,58 +709,58 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="H1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="I1" t="s">
         <v>10</v>
       </c>
       <c r="J1" t="s">
+        <v>31</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>44</v>
+      </c>
+      <c r="M1" t="s">
+        <v>39</v>
+      </c>
+      <c r="N1" t="s">
         <v>35</v>
       </c>
-      <c r="K1" t="s">
-        <v>39</v>
-      </c>
-      <c r="L1" t="s">
-        <v>50</v>
-      </c>
-      <c r="M1" t="s">
-        <v>45</v>
-      </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
+        <v>43</v>
+      </c>
+      <c r="P1" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>36</v>
+      </c>
+      <c r="R1" t="s">
+        <v>37</v>
+      </c>
+      <c r="S1" t="s">
+        <v>38</v>
+      </c>
+      <c r="T1" t="s">
+        <v>40</v>
+      </c>
+      <c r="U1" t="s">
         <v>41</v>
       </c>
-      <c r="O1" t="s">
-        <v>49</v>
-      </c>
-      <c r="P1" t="s">
-        <v>48</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>42</v>
-      </c>
-      <c r="R1" t="s">
-        <v>43</v>
-      </c>
-      <c r="S1" t="s">
-        <v>44</v>
-      </c>
-      <c r="T1" t="s">
-        <v>46</v>
-      </c>
-      <c r="U1" t="s">
-        <v>47</v>
-      </c>
       <c r="W1" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -769,16 +783,16 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>31</v>
-      </c>
-      <c r="J2" t="s">
-        <v>36</v>
+        <v>27</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L2" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M2" s="4">
         <v>37067</v>
@@ -843,10 +857,10 @@
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L3" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M3" s="4">
         <v>37384</v>
@@ -908,10 +922,10 @@
         <v>8</v>
       </c>
       <c r="K4" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L4" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M4" s="4">
         <v>35297</v>
@@ -936,7 +950,7 @@
         <v>346</v>
       </c>
       <c r="V4" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="W4">
         <v>8.67</v>
@@ -974,16 +988,16 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="J5">
         <v>7</v>
       </c>
       <c r="K5" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L5" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M5" s="4">
         <v>35668</v>
@@ -1024,84 +1038,73 @@
       </c>
     </row>
     <row r="6" spans="1:26">
-      <c r="A6" s="1">
-        <v>2427</v>
-      </c>
-      <c r="B6" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="1" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="1">
-        <v>11</v>
-      </c>
-      <c r="E6" s="1">
-        <v>1.6002000000000002E-2</v>
-      </c>
-      <c r="F6" s="1">
-        <v>1</v>
-      </c>
-      <c r="G6" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H6" s="1">
-        <v>0.5</v>
-      </c>
-      <c r="I6" s="1"/>
-      <c r="J6" s="1">
-        <v>7</v>
-      </c>
-      <c r="K6" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L6" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="M6" s="5">
-        <v>36967</v>
-      </c>
-      <c r="N6" s="5">
-        <v>37092</v>
-      </c>
-      <c r="O6" s="5">
-        <v>37092</v>
-      </c>
-      <c r="P6" s="5">
-        <v>37180</v>
-      </c>
-      <c r="Q6" s="5">
-        <v>37092</v>
-      </c>
-      <c r="R6" s="1">
+      <c r="A6">
+        <v>2151</v>
+      </c>
+      <c r="C6" t="s">
+        <v>13</v>
+      </c>
+      <c r="D6">
+        <v>9</v>
+      </c>
+      <c r="E6">
+        <v>7.9247999999999992E-3</v>
+      </c>
+      <c r="F6">
         <v>0</v>
       </c>
-      <c r="S6" s="1"/>
-      <c r="T6" s="1">
-        <v>1</v>
-      </c>
-      <c r="U6" s="1">
-        <v>211</v>
-      </c>
-      <c r="V6" s="1" t="s">
-        <v>55</v>
-      </c>
-      <c r="W6">
-        <v>3.57</v>
-      </c>
-      <c r="X6">
-        <v>10.53</v>
-      </c>
-      <c r="Y6">
-        <v>7.67</v>
-      </c>
-      <c r="Z6">
-        <v>7.67</v>
+      <c r="G6">
+        <v>0</v>
+      </c>
+      <c r="H6" t="s">
+        <v>27</v>
+      </c>
+      <c r="J6">
+        <v>3</v>
+      </c>
+      <c r="K6" t="s">
+        <v>34</v>
+      </c>
+      <c r="L6" t="s">
+        <v>47</v>
+      </c>
+      <c r="M6" s="4">
+        <v>34555</v>
+      </c>
+      <c r="N6" s="4">
+        <v>34655</v>
+      </c>
+      <c r="O6" s="4">
+        <v>34655</v>
+      </c>
+      <c r="P6" s="4">
+        <v>34655</v>
+      </c>
+      <c r="S6">
+        <v>1</v>
+      </c>
+      <c r="T6">
+        <v>1</v>
+      </c>
+      <c r="U6">
+        <v>99</v>
+      </c>
+      <c r="W6" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="X6" s="1">
+        <v>11.56</v>
+      </c>
+      <c r="Y6" s="1">
+        <v>11.56</v>
+      </c>
+      <c r="Z6" s="1">
+        <v>11.56</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="1" customFormat="1">
       <c r="A7" s="1">
-        <v>2223</v>
+        <v>2427</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>14</v>
@@ -1110,52 +1113,67 @@
         <v>15</v>
       </c>
       <c r="D7" s="1">
-        <v>69</v>
+        <v>11</v>
       </c>
       <c r="E7" s="1">
-        <v>1.2699999999999999E-2</v>
+        <v>1.6002000000000002E-2</v>
       </c>
       <c r="F7" s="1">
+        <v>1</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H7" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J7" s="1">
+        <v>7</v>
+      </c>
+      <c r="K7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L7" s="1" t="s">
+        <v>45</v>
+      </c>
+      <c r="M7" s="5">
+        <v>36967</v>
+      </c>
+      <c r="N7" s="5">
+        <v>37092</v>
+      </c>
+      <c r="O7" s="5">
+        <v>37092</v>
+      </c>
+      <c r="P7" s="5">
+        <v>37180</v>
+      </c>
+      <c r="Q7" s="5">
+        <v>37092</v>
+      </c>
+      <c r="R7" s="1">
         <v>0</v>
       </c>
-      <c r="G7" s="1">
-        <v>0</v>
-      </c>
-      <c r="H7" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J7" s="1">
-        <v>8</v>
-      </c>
-      <c r="K7" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L7" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M7" s="5">
-        <v>36623</v>
-      </c>
-      <c r="N7" s="5">
-        <v>36732</v>
-      </c>
-      <c r="O7" s="5">
-        <v>37019</v>
-      </c>
-      <c r="P7" s="5">
-        <v>37050</v>
-      </c>
-      <c r="Q7" s="5">
-        <v>36979</v>
-      </c>
-      <c r="R7" s="6">
-        <v>247</v>
-      </c>
       <c r="T7" s="1">
-        <v>280</v>
+        <v>1</v>
       </c>
       <c r="U7" s="1">
-        <v>425</v>
+        <v>211</v>
+      </c>
+      <c r="V7" s="1" t="s">
+        <v>49</v>
+      </c>
+      <c r="W7">
+        <v>3.57</v>
+      </c>
+      <c r="X7">
+        <v>10.53</v>
+      </c>
+      <c r="Y7">
+        <v>7.67</v>
+      </c>
+      <c r="Z7">
+        <v>7.67</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="1" customFormat="1">
@@ -1163,7 +1181,7 @@
         <v>2470</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="D8" s="1">
         <v>40</v>
@@ -1178,19 +1196,19 @@
         <v>0</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="I8" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="J8" s="1" t="s">
-        <v>37</v>
+        <v>17</v>
+      </c>
+      <c r="J8" s="1">
+        <v>17</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="M8" s="5">
         <v>40202</v>
@@ -1231,78 +1249,82 @@
     </row>
     <row r="9" spans="1:26" s="1" customFormat="1">
       <c r="A9" s="1">
-        <v>3120</v>
+        <v>2753</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="C9" s="1" t="s">
-        <v>23</v>
+        <v>19</v>
       </c>
       <c r="D9" s="1">
-        <v>47</v>
+        <v>91</v>
       </c>
       <c r="E9" s="1">
-        <v>9.2075000000000021E-3</v>
+        <v>8.2042E-3</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>4.7500000000000001E-2</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="H9" s="1">
-        <v>0.6</v>
+        <v>0.5</v>
       </c>
       <c r="J9" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>51</v>
+        <v>48</v>
       </c>
       <c r="M9" s="5">
-        <v>37248</v>
+        <v>36041</v>
       </c>
       <c r="N9" s="5">
-        <v>37353</v>
+        <v>36316</v>
       </c>
       <c r="O9" s="5">
-        <v>37796</v>
+        <v>36316</v>
       </c>
       <c r="P9" s="5">
-        <v>38058</v>
+        <v>36331</v>
       </c>
       <c r="Q9" s="5">
-        <v>37492</v>
-      </c>
-      <c r="R9" s="6">
-        <v>51</v>
-      </c>
+        <v>36316</v>
+      </c>
+      <c r="R9" s="1">
+        <v>0</v>
+      </c>
+      <c r="S9" s="5"/>
       <c r="T9" s="5">
-        <v>433</v>
+        <v>1</v>
       </c>
       <c r="U9" s="1">
-        <v>808</v>
+        <v>289</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="W9" s="1">
-        <v>0.76700000000000002</v>
+        <v>9.1</v>
       </c>
       <c r="X9" s="1">
-        <v>24</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="Y9" s="1">
-        <v>4.2300000000000004</v>
+        <v>18.170000000000002</v>
       </c>
       <c r="Z9" s="1">
-        <v>18.8</v>
+        <v>18.170000000000002</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="1" customFormat="1">
       <c r="A10" s="1">
-        <v>2753</v>
+        <v>3120</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
@@ -1311,330 +1333,219 @@
         <v>21</v>
       </c>
       <c r="D10" s="1">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E10" s="1">
-        <v>8.2042E-3</v>
+        <v>9.2075000000000021E-3</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>0.33600000000000002</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="H10" s="1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="J10" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="L10" s="1" t="s">
-        <v>54</v>
+        <v>45</v>
       </c>
       <c r="M10" s="5">
-        <v>36041</v>
+        <v>37248</v>
       </c>
       <c r="N10" s="5">
-        <v>36316</v>
+        <v>37353</v>
       </c>
       <c r="O10" s="5">
-        <v>36316</v>
+        <v>37796</v>
       </c>
       <c r="P10" s="5">
-        <v>36331</v>
+        <v>38058</v>
       </c>
       <c r="Q10" s="5">
-        <v>36316</v>
-      </c>
-      <c r="R10" s="1">
-        <v>0</v>
-      </c>
-      <c r="S10" s="5"/>
+        <v>37492</v>
+      </c>
+      <c r="R10" s="6">
+        <v>51</v>
+      </c>
       <c r="T10" s="5">
-        <v>1</v>
+        <v>433</v>
       </c>
       <c r="U10" s="1">
-        <v>289</v>
-      </c>
-      <c r="V10" s="1" t="s">
-        <v>58</v>
+        <v>808</v>
+      </c>
+      <c r="W10" s="1">
+        <v>0.76700000000000002</v>
+      </c>
+      <c r="X10" s="1">
+        <v>24</v>
+      </c>
+      <c r="Y10" s="1">
+        <v>4.2300000000000004</v>
+      </c>
+      <c r="Z10" s="1">
+        <v>18.8</v>
       </c>
     </row>
     <row r="11" spans="1:26" s="1" customFormat="1">
-      <c r="A11">
-        <v>2151</v>
-      </c>
-      <c r="B11"/>
-      <c r="C11" t="s">
+      <c r="A11" s="1">
+        <v>3392</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>22</v>
+      </c>
+      <c r="C11" s="1" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" s="1">
         <v>13</v>
       </c>
-      <c r="D11">
-        <v>9</v>
-      </c>
-      <c r="E11">
-        <v>7.9247999999999992E-3</v>
-      </c>
-      <c r="F11">
+      <c r="E11" s="1">
+        <v>1.00076E-2</v>
+      </c>
+      <c r="F11" s="1">
+        <v>1</v>
+      </c>
+      <c r="G11" s="1">
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="I11" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="J11" s="1">
+        <v>1</v>
+      </c>
+      <c r="K11" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="L11" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="M11" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="N11" s="5">
+        <v>37811</v>
+      </c>
+      <c r="O11" s="5">
+        <v>37811</v>
+      </c>
+      <c r="P11" s="5"/>
+      <c r="Q11" s="5">
+        <v>37811</v>
+      </c>
+      <c r="R11" s="1">
         <v>0</v>
       </c>
-      <c r="G11">
+      <c r="T11" s="5">
+        <v>1</v>
+      </c>
+      <c r="U11" s="1" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="12" spans="1:26" s="2" customFormat="1">
+      <c r="A12" s="2">
+        <v>3821</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="D12" s="2">
+        <v>73</v>
+      </c>
+      <c r="E12" s="2">
+        <v>9.5250000000000005E-3</v>
+      </c>
+      <c r="F12" s="2">
+        <v>1</v>
+      </c>
+      <c r="G12" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="H12" s="2">
+        <v>2</v>
+      </c>
+      <c r="I12" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="J12" s="2">
+        <v>1</v>
+      </c>
+      <c r="K12" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="L12" s="2" t="s">
+        <v>47</v>
+      </c>
+      <c r="M12" s="7">
+        <v>40004</v>
+      </c>
+      <c r="N12" s="7">
+        <v>40082</v>
+      </c>
+      <c r="O12" s="7">
+        <v>40082</v>
+      </c>
+      <c r="P12" s="7">
+        <v>40082</v>
+      </c>
+      <c r="Q12" s="7">
+        <v>40082</v>
+      </c>
+      <c r="R12" s="2">
         <v>0</v>
       </c>
-      <c r="H11" t="s">
-        <v>31</v>
-      </c>
-      <c r="I11"/>
-      <c r="J11">
-        <v>3</v>
-      </c>
-      <c r="K11" t="s">
-        <v>40</v>
-      </c>
-      <c r="L11" t="s">
-        <v>53</v>
-      </c>
-      <c r="M11" s="4">
-        <v>34555</v>
-      </c>
-      <c r="N11" s="4">
-        <v>34655</v>
-      </c>
-      <c r="O11" s="4">
-        <v>34655</v>
-      </c>
-      <c r="P11" s="4">
-        <v>34655</v>
-      </c>
-      <c r="Q11"/>
-      <c r="R11"/>
-      <c r="S11">
-        <v>1</v>
-      </c>
-      <c r="T11">
-        <v>1</v>
-      </c>
-      <c r="U11">
-        <v>99</v>
-      </c>
-      <c r="V11"/>
-      <c r="W11" s="1">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="X11" s="1">
-        <v>11.56</v>
-      </c>
-      <c r="Y11" s="1">
-        <v>11.56</v>
-      </c>
-      <c r="Z11" s="1">
-        <v>11.56</v>
+      <c r="T12" s="2">
+        <v>1</v>
+      </c>
+      <c r="U12" s="2">
+        <v>76</v>
+      </c>
+      <c r="W12" s="2">
+        <v>7.33</v>
+      </c>
+      <c r="X12" s="2">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="Y12" s="2">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="Z12" s="2">
+        <v>9.8699999999999992</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="1" customFormat="1">
-      <c r="A12" s="1">
-        <v>3392</v>
-      </c>
-      <c r="B12" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="1" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="1">
-        <v>13</v>
-      </c>
-      <c r="E12" s="1">
-        <v>1.00076E-2</v>
-      </c>
-      <c r="F12" s="1">
-        <v>1</v>
-      </c>
-      <c r="G12" s="1">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="H12" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="I12" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="J12" s="1">
-        <v>1</v>
-      </c>
-      <c r="K12" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L12" s="1" t="s">
-        <v>53</v>
-      </c>
-      <c r="M12" s="1" t="s">
-        <v>57</v>
-      </c>
-      <c r="N12" s="5">
-        <v>37811</v>
-      </c>
-      <c r="O12" s="5">
-        <v>37811</v>
-      </c>
-      <c r="P12" s="5"/>
-      <c r="Q12" s="5">
-        <v>37811</v>
-      </c>
-      <c r="R12" s="1">
-        <v>0</v>
-      </c>
-      <c r="T12" s="5">
-        <v>1</v>
-      </c>
-      <c r="U12" s="1" t="s">
-        <v>56</v>
-      </c>
+    <row r="13" spans="1:26">
+      <c r="A13" s="3"/>
+      <c r="D13" s="3"/>
+      <c r="F13" s="3"/>
+      <c r="G13" s="3"/>
+      <c r="H13" s="3"/>
     </row>
-    <row r="13" spans="1:26" s="1" customFormat="1">
-      <c r="A13" s="1">
-        <v>3420</v>
-      </c>
-      <c r="B13" s="1" t="s">
-        <v>26</v>
-      </c>
-      <c r="C13" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="D13" s="1">
-        <v>15</v>
-      </c>
-      <c r="E13" s="1">
-        <v>1.10998E-2</v>
-      </c>
-      <c r="F13" s="1">
-        <v>0</v>
-      </c>
-      <c r="G13" s="1">
-        <v>0</v>
-      </c>
-      <c r="H13" s="1" t="s">
-        <v>31</v>
-      </c>
-      <c r="J13" s="1">
-        <v>5</v>
-      </c>
-      <c r="K13" s="1" t="s">
-        <v>40</v>
-      </c>
-      <c r="L13" s="1" t="s">
-        <v>54</v>
-      </c>
-      <c r="M13" s="5">
-        <v>39704</v>
-      </c>
-      <c r="N13" s="5">
-        <v>39844</v>
-      </c>
-      <c r="O13" s="5">
-        <v>39856</v>
-      </c>
-      <c r="P13" s="5">
-        <v>40053</v>
-      </c>
-      <c r="T13" s="1">
-        <f>O13-N13</f>
-        <v>12</v>
-      </c>
-      <c r="U13" s="1">
-        <v>347</v>
-      </c>
-    </row>
-    <row r="14" spans="1:26" s="2" customFormat="1">
-      <c r="A14" s="2">
-        <v>3821</v>
-      </c>
-      <c r="B14" s="2" t="s">
-        <v>28</v>
-      </c>
-      <c r="C14" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="D14" s="2">
-        <v>73</v>
-      </c>
-      <c r="E14" s="2">
-        <v>9.5250000000000005E-3</v>
-      </c>
-      <c r="F14" s="2">
-        <v>1</v>
-      </c>
-      <c r="G14" s="2">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="H14" s="2">
-        <v>2</v>
-      </c>
-      <c r="I14" s="2" t="s">
-        <v>38</v>
-      </c>
-      <c r="J14" s="2">
-        <v>1</v>
-      </c>
-      <c r="K14" s="2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L14" s="2" t="s">
-        <v>53</v>
-      </c>
-      <c r="M14" s="7">
-        <v>40004</v>
-      </c>
-      <c r="N14" s="7">
-        <v>40082</v>
-      </c>
-      <c r="O14" s="7">
-        <v>40082</v>
-      </c>
-      <c r="P14" s="7">
-        <v>40082</v>
-      </c>
-      <c r="Q14" s="7">
-        <v>40082</v>
-      </c>
-      <c r="R14" s="2">
-        <v>0</v>
-      </c>
-      <c r="T14" s="2">
-        <v>1</v>
-      </c>
-      <c r="U14" s="2">
-        <v>76</v>
-      </c>
-      <c r="W14" s="2">
-        <v>7.33</v>
-      </c>
-      <c r="X14" s="2">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="Y14" s="2">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="Z14" s="2">
-        <v>9.8699999999999992</v>
-      </c>
-    </row>
-    <row r="15" spans="1:26">
-      <c r="A15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="F15" s="3"/>
-      <c r="G15" s="3"/>
-      <c r="H15" s="3"/>
-    </row>
-    <row r="16" spans="1:26">
-      <c r="D16" s="3"/>
-      <c r="F16" s="3"/>
-      <c r="G16" s="3"/>
-      <c r="H16" s="3"/>
+    <row r="14" spans="1:26">
+      <c r="D14" s="3"/>
+      <c r="F14" s="3"/>
+      <c r="G14" s="3"/>
+      <c r="H14" s="3"/>
     </row>
   </sheetData>
+  <autoFilter ref="A1:Z1">
+    <sortState ref="A2:Z12">
+      <sortCondition ref="A1:A12"/>
+    </sortState>
+  </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
   <extLst>

</xml_diff>

<commit_message>
Removed duplicate animal 1427
Now only 10 ARK cases
</commit_message>
<xml_diff>
--- a/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
+++ b/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
   <si>
     <t>Whale ID</t>
   </si>
@@ -37,12 +37,6 @@
   </si>
   <si>
     <t>Gear Length (m)</t>
-  </si>
-  <si>
-    <t>E17-02</t>
-  </si>
-  <si>
-    <t>J071202</t>
   </si>
   <si>
     <t>E9-97</t>
@@ -687,10 +681,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:Z14"/>
+  <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J9" sqref="J9"/>
+      <selection activeCell="E15" sqref="E15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -709,58 +703,58 @@
         <v>4</v>
       </c>
       <c r="E1" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="F1" t="s">
         <v>3</v>
       </c>
       <c r="G1" t="s">
+        <v>24</v>
+      </c>
+      <c r="H1" t="s">
         <v>26</v>
       </c>
-      <c r="H1" t="s">
-        <v>28</v>
-      </c>
       <c r="I1" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="J1" t="s">
+        <v>29</v>
+      </c>
+      <c r="K1" t="s">
         <v>31</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
+        <v>42</v>
+      </c>
+      <c r="M1" t="s">
+        <v>37</v>
+      </c>
+      <c r="N1" t="s">
         <v>33</v>
       </c>
-      <c r="L1" t="s">
-        <v>44</v>
-      </c>
-      <c r="M1" t="s">
+      <c r="O1" t="s">
+        <v>41</v>
+      </c>
+      <c r="P1" t="s">
+        <v>40</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>34</v>
+      </c>
+      <c r="R1" t="s">
+        <v>35</v>
+      </c>
+      <c r="S1" t="s">
+        <v>36</v>
+      </c>
+      <c r="T1" t="s">
+        <v>38</v>
+      </c>
+      <c r="U1" t="s">
         <v>39</v>
       </c>
-      <c r="N1" t="s">
-        <v>35</v>
-      </c>
-      <c r="O1" t="s">
-        <v>43</v>
-      </c>
-      <c r="P1" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>36</v>
-      </c>
-      <c r="R1" t="s">
-        <v>37</v>
-      </c>
-      <c r="S1" t="s">
-        <v>38</v>
-      </c>
-      <c r="T1" t="s">
-        <v>40</v>
-      </c>
-      <c r="U1" t="s">
-        <v>41</v>
-      </c>
       <c r="W1" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="2" spans="1:26">
@@ -768,7 +762,7 @@
         <v>1238</v>
       </c>
       <c r="C2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="D2">
         <v>88</v>
@@ -783,16 +777,16 @@
         <v>0</v>
       </c>
       <c r="H2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J2">
         <v>20</v>
       </c>
       <c r="K2" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L2" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M2" s="4">
         <v>37067</v>
@@ -830,7 +824,7 @@
     </row>
     <row r="3" spans="1:26">
       <c r="A3">
-        <v>1427</v>
+        <v>1971</v>
       </c>
       <c r="B3" t="s">
         <v>5</v>
@@ -839,147 +833,151 @@
         <v>6</v>
       </c>
       <c r="D3">
-        <v>82</v>
+        <v>88</v>
       </c>
       <c r="E3">
-        <v>1.6002000000000002E-2</v>
+        <v>1.38049E-2</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
       <c r="G3">
-        <v>0.33</v>
+        <v>0.28999999999999998</v>
       </c>
       <c r="H3">
         <v>0.5</v>
       </c>
       <c r="J3">
-        <v>18</v>
+        <v>8</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L3" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M3" s="4">
-        <v>37384</v>
-      </c>
-      <c r="N3" s="4">
-        <v>37449</v>
-      </c>
-      <c r="O3" s="4">
-        <v>37463</v>
-      </c>
+        <v>35297</v>
+      </c>
+      <c r="N3" s="8">
+        <v>35605</v>
+      </c>
+      <c r="O3" s="4"/>
       <c r="P3" s="4">
-        <v>37871</v>
-      </c>
-      <c r="T3">
-        <v>9</v>
+        <v>35643</v>
+      </c>
+      <c r="Q3" s="8">
+        <v>35605</v>
+      </c>
+      <c r="R3">
+        <v>0</v>
+      </c>
+      <c r="T3" s="6">
+        <v>22</v>
       </c>
       <c r="U3">
-        <v>485</v>
+        <v>346</v>
+      </c>
+      <c r="V3" t="s">
+        <v>44</v>
       </c>
       <c r="W3">
-        <v>5.27</v>
+        <v>8.67</v>
       </c>
       <c r="X3">
-        <v>21.23</v>
+        <v>20.03</v>
       </c>
       <c r="Y3">
-        <v>7.4</v>
+        <v>18.067</v>
       </c>
       <c r="Z3">
-        <v>7.87</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="4" spans="1:26">
       <c r="A4">
-        <v>1971</v>
+        <v>2027</v>
       </c>
       <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>10</v>
+      </c>
+      <c r="D4">
+        <v>152</v>
+      </c>
+      <c r="E4">
+        <v>1.04902E-2</v>
+      </c>
+      <c r="F4">
+        <v>0</v>
+      </c>
+      <c r="G4">
+        <v>0</v>
+      </c>
+      <c r="H4" t="s">
+        <v>25</v>
+      </c>
+      <c r="J4">
         <v>7</v>
       </c>
-      <c r="C4" t="s">
-        <v>8</v>
-      </c>
-      <c r="D4">
-        <v>88</v>
-      </c>
-      <c r="E4">
-        <v>1.38049E-2</v>
-      </c>
-      <c r="F4">
-        <v>1</v>
-      </c>
-      <c r="G4">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H4">
-        <v>0.5</v>
-      </c>
-      <c r="J4">
-        <v>8</v>
-      </c>
       <c r="K4" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M4" s="4">
-        <v>35297</v>
-      </c>
-      <c r="N4" s="8">
-        <v>35605</v>
-      </c>
-      <c r="O4" s="4"/>
+        <v>35668</v>
+      </c>
+      <c r="N4" s="4">
+        <v>35685</v>
+      </c>
+      <c r="O4" s="4">
+        <v>35685</v>
+      </c>
       <c r="P4" s="4">
-        <v>35643</v>
-      </c>
-      <c r="Q4" s="8">
-        <v>35605</v>
+        <v>35685</v>
+      </c>
+      <c r="Q4" s="4">
+        <v>35685</v>
       </c>
       <c r="R4">
         <v>0</v>
       </c>
-      <c r="T4" s="6">
-        <v>22</v>
+      <c r="T4">
+        <v>1</v>
       </c>
       <c r="U4">
-        <v>346</v>
-      </c>
-      <c r="V4" t="s">
-        <v>46</v>
-      </c>
+        <v>16</v>
+      </c>
+      <c r="V4" s="4"/>
       <c r="W4">
-        <v>8.67</v>
+        <v>8.8699999999999992</v>
       </c>
       <c r="X4">
-        <v>20.03</v>
+        <v>9.4</v>
       </c>
       <c r="Y4">
-        <v>18.067</v>
+        <v>9.4</v>
       </c>
       <c r="Z4">
-        <v>18.8</v>
+        <v>9.4</v>
       </c>
     </row>
     <row r="5" spans="1:26">
       <c r="A5">
-        <v>2027</v>
-      </c>
-      <c r="B5" t="s">
+        <v>2151</v>
+      </c>
+      <c r="C5" t="s">
         <v>11</v>
       </c>
-      <c r="C5" t="s">
-        <v>12</v>
-      </c>
       <c r="D5">
-        <v>152</v>
+        <v>9</v>
       </c>
       <c r="E5">
-        <v>1.04902E-2</v>
+        <v>7.9247999999999992E-3</v>
       </c>
       <c r="F5">
         <v>0</v>
@@ -988,168 +986,173 @@
         <v>0</v>
       </c>
       <c r="H5" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="J5">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="K5" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L5" t="s">
         <v>45</v>
       </c>
       <c r="M5" s="4">
-        <v>35668</v>
+        <v>34555</v>
       </c>
       <c r="N5" s="4">
-        <v>35685</v>
+        <v>34655</v>
       </c>
       <c r="O5" s="4">
-        <v>35685</v>
+        <v>34655</v>
       </c>
       <c r="P5" s="4">
-        <v>35685</v>
-      </c>
-      <c r="Q5" s="4">
-        <v>35685</v>
-      </c>
-      <c r="R5">
-        <v>0</v>
+        <v>34655</v>
+      </c>
+      <c r="S5">
+        <v>1</v>
       </c>
       <c r="T5">
         <v>1</v>
       </c>
       <c r="U5">
-        <v>16</v>
-      </c>
-      <c r="V5" s="4"/>
-      <c r="W5">
-        <v>8.8699999999999992</v>
-      </c>
-      <c r="X5">
-        <v>9.4</v>
-      </c>
-      <c r="Y5">
-        <v>9.4</v>
-      </c>
-      <c r="Z5">
-        <v>9.4</v>
+        <v>99</v>
+      </c>
+      <c r="W5" s="1">
+        <v>8.3000000000000007</v>
+      </c>
+      <c r="X5" s="1">
+        <v>11.56</v>
+      </c>
+      <c r="Y5" s="1">
+        <v>11.56</v>
+      </c>
+      <c r="Z5" s="1">
+        <v>11.56</v>
       </c>
     </row>
-    <row r="6" spans="1:26">
-      <c r="A6">
-        <v>2151</v>
-      </c>
-      <c r="C6" t="s">
+    <row r="6" spans="1:26" s="1" customFormat="1">
+      <c r="A6" s="1">
+        <v>2427</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="D6">
-        <v>9</v>
-      </c>
-      <c r="E6">
-        <v>7.9247999999999992E-3</v>
-      </c>
-      <c r="F6">
-        <v>0</v>
-      </c>
-      <c r="G6">
-        <v>0</v>
-      </c>
-      <c r="H6" t="s">
-        <v>27</v>
-      </c>
-      <c r="J6">
-        <v>3</v>
-      </c>
-      <c r="K6" t="s">
-        <v>34</v>
-      </c>
-      <c r="L6" t="s">
+      <c r="D6" s="1">
+        <v>11</v>
+      </c>
+      <c r="E6" s="1">
+        <v>1.6002000000000002E-2</v>
+      </c>
+      <c r="F6" s="1">
+        <v>1</v>
+      </c>
+      <c r="G6" s="1">
+        <v>0.28999999999999998</v>
+      </c>
+      <c r="H6" s="1">
+        <v>0.5</v>
+      </c>
+      <c r="J6" s="1">
+        <v>7</v>
+      </c>
+      <c r="K6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L6" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="M6" s="5">
+        <v>36967</v>
+      </c>
+      <c r="N6" s="5">
+        <v>37092</v>
+      </c>
+      <c r="O6" s="5">
+        <v>37092</v>
+      </c>
+      <c r="P6" s="5">
+        <v>37180</v>
+      </c>
+      <c r="Q6" s="5">
+        <v>37092</v>
+      </c>
+      <c r="R6" s="1">
+        <v>0</v>
+      </c>
+      <c r="T6" s="1">
+        <v>1</v>
+      </c>
+      <c r="U6" s="1">
+        <v>211</v>
+      </c>
+      <c r="V6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="M6" s="4">
-        <v>34555</v>
-      </c>
-      <c r="N6" s="4">
-        <v>34655</v>
-      </c>
-      <c r="O6" s="4">
-        <v>34655</v>
-      </c>
-      <c r="P6" s="4">
-        <v>34655</v>
-      </c>
-      <c r="S6">
-        <v>1</v>
-      </c>
-      <c r="T6">
-        <v>1</v>
-      </c>
-      <c r="U6">
-        <v>99</v>
-      </c>
-      <c r="W6" s="1">
-        <v>8.3000000000000007</v>
-      </c>
-      <c r="X6" s="1">
-        <v>11.56</v>
-      </c>
-      <c r="Y6" s="1">
-        <v>11.56</v>
-      </c>
-      <c r="Z6" s="1">
-        <v>11.56</v>
+      <c r="W6">
+        <v>3.57</v>
+      </c>
+      <c r="X6">
+        <v>10.53</v>
+      </c>
+      <c r="Y6">
+        <v>7.67</v>
+      </c>
+      <c r="Z6">
+        <v>7.67</v>
       </c>
     </row>
     <row r="7" spans="1:26" s="1" customFormat="1">
       <c r="A7" s="1">
-        <v>2427</v>
-      </c>
-      <c r="B7" s="1" t="s">
+        <v>2470</v>
+      </c>
+      <c r="C7" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="C7" s="1" t="s">
+      <c r="D7" s="1">
+        <v>40</v>
+      </c>
+      <c r="E7" s="1">
+        <v>1.6560800000000001E-2</v>
+      </c>
+      <c r="F7" s="1">
+        <v>0</v>
+      </c>
+      <c r="G7" s="1">
+        <v>0</v>
+      </c>
+      <c r="H7" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="I7" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="1">
-        <v>11</v>
-      </c>
-      <c r="E7" s="1">
-        <v>1.6002000000000002E-2</v>
-      </c>
-      <c r="F7" s="1">
-        <v>1</v>
-      </c>
-      <c r="G7" s="1">
-        <v>0.28999999999999998</v>
-      </c>
-      <c r="H7" s="1">
-        <v>0.5</v>
-      </c>
       <c r="J7" s="1">
-        <v>7</v>
+        <v>17</v>
       </c>
       <c r="K7" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L7" s="1" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="M7" s="5">
-        <v>36967</v>
+        <v>40202</v>
       </c>
       <c r="N7" s="5">
-        <v>37092</v>
+        <v>40311</v>
       </c>
       <c r="O7" s="5">
-        <v>37092</v>
+        <v>40311</v>
       </c>
       <c r="P7" s="5">
-        <v>37180</v>
+        <v>40311</v>
       </c>
       <c r="Q7" s="5">
-        <v>37092</v>
+        <v>40311</v>
       </c>
       <c r="R7" s="1">
         <v>0</v>
@@ -1158,98 +1161,99 @@
         <v>1</v>
       </c>
       <c r="U7" s="1">
-        <v>211</v>
-      </c>
-      <c r="V7" s="1" t="s">
-        <v>49</v>
-      </c>
-      <c r="W7">
-        <v>3.57</v>
-      </c>
-      <c r="X7">
-        <v>10.53</v>
-      </c>
-      <c r="Y7">
-        <v>7.67</v>
-      </c>
-      <c r="Z7">
-        <v>7.67</v>
+        <v>106</v>
+      </c>
+      <c r="W7" s="1">
+        <v>1.8</v>
+      </c>
+      <c r="X7" s="1">
+        <v>5.43</v>
+      </c>
+      <c r="Y7" s="1">
+        <v>5.43</v>
+      </c>
+      <c r="Z7" s="1">
+        <v>5.43</v>
       </c>
     </row>
     <row r="8" spans="1:26" s="1" customFormat="1">
       <c r="A8" s="1">
-        <v>2470</v>
+        <v>2753</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>16</v>
       </c>
       <c r="C8" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="D8" s="1">
-        <v>40</v>
+        <v>91</v>
       </c>
       <c r="E8" s="1">
-        <v>1.6560800000000001E-2</v>
+        <v>8.2042E-3</v>
       </c>
       <c r="F8" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="G8" s="1">
-        <v>0</v>
-      </c>
-      <c r="H8" s="1" t="s">
-        <v>27</v>
-      </c>
-      <c r="I8" s="1" t="s">
-        <v>17</v>
+        <v>0.33600000000000002</v>
+      </c>
+      <c r="H8" s="1">
+        <v>0.5</v>
       </c>
       <c r="J8" s="1">
-        <v>17</v>
+        <v>2</v>
       </c>
       <c r="K8" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L8" s="1" t="s">
-        <v>45</v>
+        <v>46</v>
       </c>
       <c r="M8" s="5">
-        <v>40202</v>
+        <v>36041</v>
       </c>
       <c r="N8" s="5">
-        <v>40311</v>
+        <v>36316</v>
       </c>
       <c r="O8" s="5">
-        <v>40311</v>
+        <v>36316</v>
       </c>
       <c r="P8" s="5">
-        <v>40311</v>
+        <v>36331</v>
       </c>
       <c r="Q8" s="5">
-        <v>40311</v>
+        <v>36316</v>
       </c>
       <c r="R8" s="1">
         <v>0</v>
       </c>
-      <c r="T8" s="1">
+      <c r="S8" s="5"/>
+      <c r="T8" s="5">
         <v>1</v>
       </c>
       <c r="U8" s="1">
-        <v>106</v>
+        <v>289</v>
+      </c>
+      <c r="V8" s="1" t="s">
+        <v>50</v>
       </c>
       <c r="W8" s="1">
-        <v>1.8</v>
+        <v>9.1</v>
       </c>
       <c r="X8" s="1">
-        <v>5.43</v>
+        <v>18.670000000000002</v>
       </c>
       <c r="Y8" s="1">
-        <v>5.43</v>
+        <v>18.170000000000002</v>
       </c>
       <c r="Z8" s="1">
-        <v>5.43</v>
+        <v>18.170000000000002</v>
       </c>
     </row>
     <row r="9" spans="1:26" s="1" customFormat="1">
       <c r="A9" s="1">
-        <v>2753</v>
+        <v>3120</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>18</v>
@@ -1258,73 +1262,69 @@
         <v>19</v>
       </c>
       <c r="D9" s="1">
-        <v>91</v>
+        <v>47</v>
       </c>
       <c r="E9" s="1">
-        <v>8.2042E-3</v>
+        <v>9.2075000000000021E-3</v>
       </c>
       <c r="F9" s="1">
         <v>1</v>
       </c>
       <c r="G9" s="1">
-        <v>0.33600000000000002</v>
+        <v>4.7500000000000001E-2</v>
       </c>
       <c r="H9" s="1">
-        <v>0.5</v>
+        <v>0.6</v>
       </c>
       <c r="J9" s="1">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="K9" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L9" s="1" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="M9" s="5">
-        <v>36041</v>
+        <v>37248</v>
       </c>
       <c r="N9" s="5">
-        <v>36316</v>
+        <v>37353</v>
       </c>
       <c r="O9" s="5">
-        <v>36316</v>
+        <v>37796</v>
       </c>
       <c r="P9" s="5">
-        <v>36331</v>
+        <v>38058</v>
       </c>
       <c r="Q9" s="5">
-        <v>36316</v>
-      </c>
-      <c r="R9" s="1">
-        <v>0</v>
-      </c>
-      <c r="S9" s="5"/>
+        <v>37492</v>
+      </c>
+      <c r="R9" s="6">
+        <v>51</v>
+      </c>
       <c r="T9" s="5">
-        <v>1</v>
+        <v>433</v>
       </c>
       <c r="U9" s="1">
-        <v>289</v>
-      </c>
-      <c r="V9" s="1" t="s">
-        <v>52</v>
+        <v>808</v>
       </c>
       <c r="W9" s="1">
-        <v>9.1</v>
+        <v>0.76700000000000002</v>
       </c>
       <c r="X9" s="1">
-        <v>18.670000000000002</v>
+        <v>24</v>
       </c>
       <c r="Y9" s="1">
-        <v>18.170000000000002</v>
+        <v>4.2300000000000004</v>
       </c>
       <c r="Z9" s="1">
-        <v>18.170000000000002</v>
+        <v>18.8</v>
       </c>
     </row>
     <row r="10" spans="1:26" s="1" customFormat="1">
       <c r="A10" s="1">
-        <v>3120</v>
+        <v>3392</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>20</v>
@@ -1333,212 +1333,141 @@
         <v>21</v>
       </c>
       <c r="D10" s="1">
-        <v>47</v>
+        <v>13</v>
       </c>
       <c r="E10" s="1">
-        <v>9.2075000000000021E-3</v>
+        <v>1.00076E-2</v>
       </c>
       <c r="F10" s="1">
         <v>1</v>
       </c>
       <c r="G10" s="1">
-        <v>4.7500000000000001E-2</v>
+        <v>0.33600000000000002</v>
       </c>
       <c r="H10" s="1">
-        <v>0.6</v>
+        <v>1.8</v>
+      </c>
+      <c r="I10" s="1" t="s">
+        <v>28</v>
       </c>
       <c r="J10" s="1">
         <v>1</v>
       </c>
       <c r="K10" s="1" t="s">
-        <v>34</v>
+        <v>32</v>
       </c>
       <c r="L10" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="M10" s="5">
-        <v>37248</v>
+      <c r="M10" s="1" t="s">
+        <v>49</v>
       </c>
       <c r="N10" s="5">
-        <v>37353</v>
+        <v>37811</v>
       </c>
       <c r="O10" s="5">
-        <v>37796</v>
-      </c>
-      <c r="P10" s="5">
-        <v>38058</v>
-      </c>
+        <v>37811</v>
+      </c>
+      <c r="P10" s="5"/>
       <c r="Q10" s="5">
-        <v>37492</v>
-      </c>
-      <c r="R10" s="6">
-        <v>51</v>
+        <v>37811</v>
+      </c>
+      <c r="R10" s="1">
+        <v>0</v>
       </c>
       <c r="T10" s="5">
-        <v>433</v>
-      </c>
-      <c r="U10" s="1">
-        <v>808</v>
-      </c>
-      <c r="W10" s="1">
-        <v>0.76700000000000002</v>
-      </c>
-      <c r="X10" s="1">
-        <v>24</v>
-      </c>
-      <c r="Y10" s="1">
-        <v>4.2300000000000004</v>
-      </c>
-      <c r="Z10" s="1">
-        <v>18.8</v>
+        <v>1</v>
+      </c>
+      <c r="U10" s="1" t="s">
+        <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="1" customFormat="1">
-      <c r="A11" s="1">
-        <v>3392</v>
-      </c>
-      <c r="B11" s="1" t="s">
+    <row r="11" spans="1:26" s="2" customFormat="1">
+      <c r="A11" s="2">
+        <v>3821</v>
+      </c>
+      <c r="B11" s="2" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="1" t="s">
+      <c r="C11" s="2" t="s">
         <v>23</v>
       </c>
-      <c r="D11" s="1">
-        <v>13</v>
-      </c>
-      <c r="E11" s="1">
-        <v>1.00076E-2</v>
-      </c>
-      <c r="F11" s="1">
-        <v>1</v>
-      </c>
-      <c r="G11" s="1">
-        <v>0.33600000000000002</v>
-      </c>
-      <c r="H11" s="1">
-        <v>1.8</v>
-      </c>
-      <c r="I11" s="1" t="s">
+      <c r="D11" s="2">
+        <v>73</v>
+      </c>
+      <c r="E11" s="2">
+        <v>9.5250000000000005E-3</v>
+      </c>
+      <c r="F11" s="2">
+        <v>1</v>
+      </c>
+      <c r="G11" s="2">
+        <v>0.30399999999999999</v>
+      </c>
+      <c r="H11" s="2">
+        <v>2</v>
+      </c>
+      <c r="I11" s="2" t="s">
         <v>30</v>
       </c>
-      <c r="J11" s="1">
-        <v>1</v>
-      </c>
-      <c r="K11" s="1" t="s">
-        <v>34</v>
-      </c>
-      <c r="L11" s="1" t="s">
-        <v>47</v>
-      </c>
-      <c r="M11" s="1" t="s">
-        <v>51</v>
-      </c>
-      <c r="N11" s="5">
-        <v>37811</v>
-      </c>
-      <c r="O11" s="5">
-        <v>37811</v>
-      </c>
-      <c r="P11" s="5"/>
-      <c r="Q11" s="5">
-        <v>37811</v>
-      </c>
-      <c r="R11" s="1">
-        <v>0</v>
-      </c>
-      <c r="T11" s="5">
-        <v>1</v>
-      </c>
-      <c r="U11" s="1" t="s">
-        <v>50</v>
+      <c r="J11" s="2">
+        <v>1</v>
+      </c>
+      <c r="K11" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="L11" s="2" t="s">
+        <v>45</v>
+      </c>
+      <c r="M11" s="7">
+        <v>40004</v>
+      </c>
+      <c r="N11" s="7">
+        <v>40082</v>
+      </c>
+      <c r="O11" s="7">
+        <v>40082</v>
+      </c>
+      <c r="P11" s="7">
+        <v>40082</v>
+      </c>
+      <c r="Q11" s="7">
+        <v>40082</v>
+      </c>
+      <c r="R11" s="2">
+        <v>0</v>
+      </c>
+      <c r="T11" s="2">
+        <v>1</v>
+      </c>
+      <c r="U11" s="2">
+        <v>76</v>
+      </c>
+      <c r="W11" s="2">
+        <v>7.33</v>
+      </c>
+      <c r="X11" s="2">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="Y11" s="2">
+        <v>9.8699999999999992</v>
+      </c>
+      <c r="Z11" s="2">
+        <v>9.8699999999999992</v>
       </c>
     </row>
-    <row r="12" spans="1:26" s="2" customFormat="1">
-      <c r="A12" s="2">
-        <v>3821</v>
-      </c>
-      <c r="B12" s="2" t="s">
-        <v>24</v>
-      </c>
-      <c r="C12" s="2" t="s">
-        <v>25</v>
-      </c>
-      <c r="D12" s="2">
-        <v>73</v>
-      </c>
-      <c r="E12" s="2">
-        <v>9.5250000000000005E-3</v>
-      </c>
-      <c r="F12" s="2">
-        <v>1</v>
-      </c>
-      <c r="G12" s="2">
-        <v>0.30399999999999999</v>
-      </c>
-      <c r="H12" s="2">
-        <v>2</v>
-      </c>
-      <c r="I12" s="2" t="s">
-        <v>32</v>
-      </c>
-      <c r="J12" s="2">
-        <v>1</v>
-      </c>
-      <c r="K12" s="2" t="s">
-        <v>34</v>
-      </c>
-      <c r="L12" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="M12" s="7">
-        <v>40004</v>
-      </c>
-      <c r="N12" s="7">
-        <v>40082</v>
-      </c>
-      <c r="O12" s="7">
-        <v>40082</v>
-      </c>
-      <c r="P12" s="7">
-        <v>40082</v>
-      </c>
-      <c r="Q12" s="7">
-        <v>40082</v>
-      </c>
-      <c r="R12" s="2">
-        <v>0</v>
-      </c>
-      <c r="T12" s="2">
-        <v>1</v>
-      </c>
-      <c r="U12" s="2">
-        <v>76</v>
-      </c>
-      <c r="W12" s="2">
-        <v>7.33</v>
-      </c>
-      <c r="X12" s="2">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="Y12" s="2">
-        <v>9.8699999999999992</v>
-      </c>
-      <c r="Z12" s="2">
-        <v>9.8699999999999992</v>
-      </c>
+    <row r="12" spans="1:26">
+      <c r="A12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="F12" s="3"/>
+      <c r="G12" s="3"/>
+      <c r="H12" s="3"/>
     </row>
     <row r="13" spans="1:26">
-      <c r="A13" s="3"/>
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
       <c r="H13" s="3"/>
-    </row>
-    <row r="14" spans="1:26">
-      <c r="D14" s="3"/>
-      <c r="F14" s="3"/>
-      <c r="G14" s="3"/>
-      <c r="H14" s="3"/>
     </row>
   </sheetData>
   <autoFilter ref="A1:Z1">

</xml_diff>

<commit_message>
Plotting, presentation, 2017 Snow Crab Data
</commit_message>
<xml_diff>
--- a/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
+++ b/DragTheoryComparison/ARK_CaseStudiestoUse.xlsx
@@ -1,10 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="26122"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="5" rupBuild="27309"/>
   <workbookPr showInkAnnotation="0" autoCompressPictures="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/julievanderhoop/Documents/MATLAB/TOW/DragTheoryComparison/"/>
+    </mc:Choice>
+  </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="240" yWindow="240" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
+    <workbookView xWindow="240" yWindow="460" windowWidth="25360" windowHeight="14640" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -12,8 +17,11 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$Z$1</definedName>
   </definedNames>
-  <calcPr calcId="140000" concurrentCalc="0"/>
+  <calcPr calcId="150001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{79F54976-1DA5-4618-B147-4CDE4B953A38}">
+      <x14:workbookPr defaultImageDpi="32767"/>
+    </ext>
     <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
       <mx:ArchID Flags="2"/>
     </ext>
@@ -22,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="71" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="53">
   <si>
     <t>Whale ID</t>
   </si>
@@ -178,6 +186,9 @@
   </si>
   <si>
     <t>Entang Matrix</t>
+  </si>
+  <si>
+    <t>Amy's report says 808, but 433 days since LSGF</t>
   </si>
 </sst>
 </file>
@@ -241,7 +252,7 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="49">
+  <cellStyleXfs count="53">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
@@ -291,8 +302,12 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -302,8 +317,9 @@
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="15" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="15" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="49">
+  <cellStyles count="53">
     <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="6" builtinId="9" hidden="1"/>
@@ -328,6 +344,8 @@
     <cellStyle name="Followed Hyperlink" xfId="44" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="46" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="48" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="50" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="52" builtinId="9" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="5" builtinId="8" hidden="1"/>
@@ -352,10 +370,17 @@
     <cellStyle name="Hyperlink" xfId="43" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="45" builtinId="8" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="47" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="49" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="51" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleMedium4"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -684,12 +709,12 @@
   <dimension ref="A1:Z13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E15" sqref="E15"/>
+      <selection activeCell="G21" sqref="G21:G23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="1" spans="1:26">
+    <row r="1" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -757,7 +782,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="2" spans="1:26">
+    <row r="2" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1238</v>
       </c>
@@ -822,7 +847,7 @@
         <v>10.83</v>
       </c>
     </row>
-    <row r="3" spans="1:26">
+    <row r="3" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1971</v>
       </c>
@@ -872,6 +897,9 @@
       <c r="R3">
         <v>0</v>
       </c>
+      <c r="S3">
+        <v>0</v>
+      </c>
       <c r="T3" s="6">
         <v>22</v>
       </c>
@@ -894,7 +922,7 @@
         <v>18.8</v>
       </c>
     </row>
-    <row r="4" spans="1:26">
+    <row r="4" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2027</v>
       </c>
@@ -944,6 +972,9 @@
         <v>35685</v>
       </c>
       <c r="R4">
+        <v>0</v>
+      </c>
+      <c r="S4" s="4">
         <v>0</v>
       </c>
       <c r="T4">
@@ -966,7 +997,7 @@
         <v>9.4</v>
       </c>
     </row>
-    <row r="5" spans="1:26">
+    <row r="5" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>2151</v>
       </c>
@@ -1031,7 +1062,7 @@
         <v>11.56</v>
       </c>
     </row>
-    <row r="6" spans="1:26" s="1" customFormat="1">
+    <row r="6" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A6" s="1">
         <v>2427</v>
       </c>
@@ -1083,6 +1114,9 @@
       <c r="R6" s="1">
         <v>0</v>
       </c>
+      <c r="S6" s="5">
+        <v>0</v>
+      </c>
       <c r="T6" s="1">
         <v>1</v>
       </c>
@@ -1105,7 +1139,7 @@
         <v>7.67</v>
       </c>
     </row>
-    <row r="7" spans="1:26" s="1" customFormat="1">
+    <row r="7" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A7" s="1">
         <v>2470</v>
       </c>
@@ -1157,6 +1191,9 @@
       <c r="R7" s="1">
         <v>0</v>
       </c>
+      <c r="S7" s="5">
+        <v>0</v>
+      </c>
       <c r="T7" s="1">
         <v>1</v>
       </c>
@@ -1176,7 +1213,7 @@
         <v>5.43</v>
       </c>
     </row>
-    <row r="8" spans="1:26" s="1" customFormat="1">
+    <row r="8" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A8" s="1">
         <v>2753</v>
       </c>
@@ -1228,8 +1265,10 @@
       <c r="R8" s="1">
         <v>0</v>
       </c>
-      <c r="S8" s="5"/>
-      <c r="T8" s="5">
+      <c r="S8" s="5">
+        <v>0</v>
+      </c>
+      <c r="T8" s="9">
         <v>1</v>
       </c>
       <c r="U8" s="1">
@@ -1251,7 +1290,7 @@
         <v>18.170000000000002</v>
       </c>
     </row>
-    <row r="9" spans="1:26" s="1" customFormat="1">
+    <row r="9" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A9" s="1">
         <v>3120</v>
       </c>
@@ -1295,7 +1334,7 @@
         <v>37796</v>
       </c>
       <c r="P9" s="5">
-        <v>38058</v>
+        <v>38245</v>
       </c>
       <c r="Q9" s="5">
         <v>37492</v>
@@ -1303,11 +1342,18 @@
       <c r="R9" s="6">
         <v>51</v>
       </c>
-      <c r="T9" s="5">
+      <c r="S9" s="5">
+        <v>0</v>
+      </c>
+      <c r="T9" s="9">
         <v>433</v>
       </c>
       <c r="U9" s="1">
-        <v>808</v>
+        <f>P9-M9</f>
+        <v>997</v>
+      </c>
+      <c r="V9" s="1" t="s">
+        <v>52</v>
       </c>
       <c r="W9" s="1">
         <v>0.76700000000000002</v>
@@ -1319,10 +1365,10 @@
         <v>4.2300000000000004</v>
       </c>
       <c r="Z9" s="1">
-        <v>18.8</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="10" spans="1:26" s="1" customFormat="1">
+    <row r="10" spans="1:26" s="1" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A10" s="1">
         <v>3392</v>
       </c>
@@ -1375,14 +1421,17 @@
       <c r="R10" s="1">
         <v>0</v>
       </c>
-      <c r="T10" s="5">
+      <c r="S10" s="5">
+        <v>0</v>
+      </c>
+      <c r="T10" s="9">
         <v>1</v>
       </c>
       <c r="U10" s="1" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="11" spans="1:26" s="2" customFormat="1">
+    <row r="11" spans="1:26" s="2" customFormat="1" x14ac:dyDescent="0.2">
       <c r="A11" s="2">
         <v>3821</v>
       </c>
@@ -1437,6 +1486,9 @@
       <c r="R11" s="2">
         <v>0</v>
       </c>
+      <c r="S11" s="2">
+        <v>0</v>
+      </c>
       <c r="T11" s="2">
         <v>1</v>
       </c>
@@ -1456,14 +1508,14 @@
         <v>9.8699999999999992</v>
       </c>
     </row>
-    <row r="12" spans="1:26">
+    <row r="12" spans="1:26" x14ac:dyDescent="0.2">
       <c r="A12" s="3"/>
       <c r="D12" s="3"/>
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
       <c r="H12" s="3"/>
     </row>
-    <row r="13" spans="1:26">
+    <row r="13" spans="1:26" x14ac:dyDescent="0.2">
       <c r="D13" s="3"/>
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
@@ -1477,10 +1529,5 @@
   </autoFilter>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>
-  <extLst>
-    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
-      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
-    </ext>
-  </extLst>
 </worksheet>
 </file>
</xml_diff>